<commit_message>
colour-coding extra-fields, not mandatory
</commit_message>
<xml_diff>
--- a/sample-files/tailored-templates/sample-template.xlsx
+++ b/sample-files/tailored-templates/sample-template.xlsx
@@ -110,7 +110,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,13 +120,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFF9AE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFBD7CB5"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF9AE"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -171,7 +177,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -188,7 +194,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,7 +218,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -221,7 +231,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFF9AE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -250,7 +260,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFBD7CB5"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -272,7 +282,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -331,10 +341,10 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>